<commit_message>
finished the first project
</commit_message>
<xml_diff>
--- a/first-neural-network/超参数实验结果.xlsx
+++ b/first-neural-network/超参数实验结果.xlsx
@@ -69,12 +69,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -89,8 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -371,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:I10"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -388,7 +395,7 @@
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -411,7 +418,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>5000</v>
       </c>
@@ -434,7 +441,7 @@
         <v>0.14099999999999999</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>5000</v>
       </c>
@@ -457,7 +464,7 @@
         <v>0.20799999999999999</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>5000</v>
       </c>
@@ -480,7 +487,7 @@
         <v>0.14399999999999999</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>5000</v>
       </c>
@@ -503,7 +510,7 @@
         <v>0.74199999999999999</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>50000</v>
       </c>
@@ -526,7 +533,7 @@
         <v>0.14899999999999999</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>50000</v>
       </c>
@@ -549,7 +556,7 @@
         <v>0.13800000000000001</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>50000</v>
       </c>
@@ -572,35 +579,37 @@
         <v>0.16900000000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1">
         <v>50000</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="1">
         <v>0.5</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>8</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>128</v>
-      </c>
-      <c r="H9">
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>128</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1">
         <v>0.05</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="1">
         <v>0.124</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>50000</v>
+        <v>10000</v>
       </c>
       <c r="C10">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="D10">
         <v>8</v>
@@ -612,10 +621,102 @@
         <v>128</v>
       </c>
       <c r="H10">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="I10">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>100000</v>
+      </c>
+      <c r="C11">
+        <v>0.5</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>128</v>
+      </c>
+      <c r="H11">
+        <v>4.7E-2</v>
+      </c>
+      <c r="I11">
+        <v>0.154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>50000</v>
+      </c>
+      <c r="C12">
+        <v>0.3</v>
+      </c>
+      <c r="D12">
+        <v>8</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>128</v>
+      </c>
+      <c r="H12">
         <v>0.05</v>
       </c>
-      <c r="I10">
+      <c r="I12">
         <v>0.19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>50000</v>
+      </c>
+      <c r="C13">
+        <v>0.3</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>128</v>
+      </c>
+      <c r="H13">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="I13">
+        <v>0.154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>100000</v>
+      </c>
+      <c r="C14">
+        <v>0.1</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>128</v>
+      </c>
+      <c r="H14">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="I14">
+        <v>0.219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>